<commit_message>
Se implemento las notificaciones de cocina a bar
</commit_message>
<xml_diff>
--- a/data/Ventas_Entradas.xlsx
+++ b/data/Ventas_Entradas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,100 +454,6 @@
           <t>Total_Venta</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Fecha</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Hora</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Adultos</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Niños</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Tercera_Edad</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Detalle</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="n">
-        <v>6</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2025-03-12</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>17:19:53</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>prueba1</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="n">
-        <v>50</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2025-03-12</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>17:20:28</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>5</v>
-      </c>
-      <c r="H3" t="n">
-        <v>3</v>
-      </c>
-      <c r="I3" t="n">
-        <v>2</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>prueba2</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>